<commit_message>
MathStat idz 2,3 reports
</commit_message>
<xml_diff>
--- a/2COURSE/2SEM/MathStat/tasks/task3/idz3_var93.xlsx
+++ b/2COURSE/2SEM/MathStat/tasks/task3/idz3_var93.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graev\OneDrive\Рабочий стол\ITMO\2COURSE\2SEM\MathStat\tasks\task3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0949E866-F80F-49D1-BD65-C31C2E271CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419A8CDE-F6A1-4CDA-934F-2825CDDBF998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{D2A8B818-9812-4144-89C5-94F18FA9520B}"/>
   </bookViews>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397BA641-7112-4114-AB74-D5183F7DAE32}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="W40" sqref="W40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,7 +1196,7 @@
         <v>0.95</v>
       </c>
       <c r="P39" s="1">
-        <v>2.0848</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="D44" s="1">
         <f>P39</f>
-        <v>2.0848</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">

</xml_diff>